<commit_message>
with new adance update with jenkins and profiling
</commit_message>
<xml_diff>
--- a/ComcastCRMGUIFramework/testData/testScriptData.xlsx
+++ b/ComcastCRMGUIFramework/testData/testScriptData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINIT SINGH\Desktop\Tek Pyramid\selenium practice\ComcastCRMGUIFramework\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINIT SINGH\git\AutomationLead\ComcastCRMGUIFramework\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BE4D5D-D268-4496-94F3-39163FE473C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83062491-78C3-41E2-BDD3-AD5970084E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
@@ -528,12 +528,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD30963-50BE-4983-A8BE-05C393FA8513}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -971,34 +970,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>